<commit_message>
change logo, update workout routines
</commit_message>
<xml_diff>
--- a/static/workouts.xlsx
+++ b/static/workouts.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cgrant/Library/CloudStorage/OneDrive-Personal/GitHub/geocoug/toolkit/static/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/54d68f46f5829c2c/GitHub/geocoug/toolkit/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59253BDA-01CC-C142-B312-A4B0FDFD7281}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{59253BDA-01CC-C142-B312-A4B0FDFD7281}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D516BEBD-77B8-1148-AFF5-BE26CFD536BE}"/>
   <bookViews>
-    <workbookView xWindow="20560" yWindow="880" windowWidth="20560" windowHeight="24260" activeTab="3" xr2:uid="{33B94D11-EE83-ED43-B23D-BCAC305DFE17}"/>
+    <workbookView xWindow="20560" yWindow="880" windowWidth="20560" windowHeight="24260" activeTab="1" xr2:uid="{33B94D11-EE83-ED43-B23D-BCAC305DFE17}"/>
   </bookViews>
   <sheets>
     <sheet name="Back-Biceps-Abs" sheetId="1" r:id="rId1"/>
@@ -139,9 +139,6 @@
     <t>Kettlebell Swing</t>
   </si>
   <si>
-    <t>Dumbbell Shrugs</t>
-  </si>
-  <si>
     <t>Barbell Shrugs</t>
   </si>
   <si>
@@ -158,6 +155,9 @@
   </si>
   <si>
     <t>Farmers Carry</t>
+  </si>
+  <si>
+    <t>Dumbbell Press</t>
   </si>
 </sst>
 </file>
@@ -509,11 +509,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CF3C11C-73CE-304C-B13C-F9FD3DC9A2A4}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -607,34 +605,45 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="B9">
-        <v>3</v>
-      </c>
-      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9">
         <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B10">
         <v>3</v>
       </c>
-      <c r="C10">
-        <v>15</v>
+      <c r="C10" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="C11">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>14</v>
       </c>
-      <c r="B11">
-        <v>3</v>
-      </c>
-      <c r="C11">
+      <c r="B12">
+        <v>3</v>
+      </c>
+      <c r="C12">
         <v>25</v>
       </c>
     </row>
@@ -647,8 +656,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B4E81E3-F197-394F-B96A-34A73554A4BF}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -721,7 +730,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="B7">
         <v>4</v>
@@ -732,18 +741,18 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B8">
         <v>3</v>
       </c>
       <c r="C8">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B9">
         <v>3</v>
@@ -762,7 +771,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -791,7 +800,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B3">
         <v>4</v>
@@ -824,7 +833,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B6">
         <v>4</v>
@@ -862,11 +871,9 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BF8F0F7-407A-0C45-9397-8FA0C20E56A9}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -927,7 +934,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B6">
         <v>4</v>
@@ -960,23 +967,12 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B9">
         <v>3</v>
       </c>
-      <c r="C9">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>39</v>
-      </c>
-      <c r="B10">
-        <v>3</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="C9" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>